<commit_message>
add functionality for rsm
</commit_message>
<xml_diff>
--- a/Data/Call/Call_CBU.xlsx
+++ b/Data/Call/Call_CBU.xlsx
@@ -82,9 +82,6 @@
     <t>CBU32</t>
   </si>
   <si>
-    <t>CBU33</t>
-  </si>
-  <si>
     <t>CBU34</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>CBU45</t>
+  </si>
+  <si>
+    <t>CBU46</t>
   </si>
   <si>
     <t>CBU52</t>
@@ -555,31 +555,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -590,28 +590,28 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>8</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -619,31 +619,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -651,31 +651,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -683,31 +683,31 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -715,31 +715,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -747,31 +747,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -779,31 +779,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
       <c r="H9">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -811,31 +811,31 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H10">
         <v>7</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -843,31 +843,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -875,31 +875,31 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
         <v>19</v>
       </c>
-      <c r="G12">
-        <v>22</v>
-      </c>
       <c r="H12">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -907,31 +907,31 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -939,22 +939,22 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G14">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>12</v>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -971,31 +971,31 @@
         <v>23</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
         <v>8</v>
       </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>16</v>
-      </c>
-      <c r="H15">
-        <v>15</v>
-      </c>
       <c r="I15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1003,13 +1003,13 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1018,16 +1018,16 @@
         <v>4</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1035,31 +1035,31 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <v>2</v>
       </c>
       <c r="J17">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1067,31 +1067,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18">
         <v>9</v>
       </c>
       <c r="G18">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J18">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1099,31 +1099,31 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1131,31 +1131,31 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G20">
         <v>4</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1163,31 +1163,31 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21">
         <v>11</v>
       </c>
-      <c r="F21">
-        <v>14</v>
-      </c>
-      <c r="G21">
-        <v>13</v>
-      </c>
       <c r="H21">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1195,31 +1195,31 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1227,31 +1227,31 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1259,10 +1259,10 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1271,19 +1271,19 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1291,28 +1291,28 @@
         <v>33</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H25">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1323,31 +1323,31 @@
         <v>34</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1355,31 +1355,31 @@
         <v>35</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>5</v>
       </c>
       <c r="G27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1387,31 +1387,31 @@
         <v>36</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G28">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1422,28 +1422,28 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1451,31 +1451,31 @@
         <v>38</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1483,31 +1483,31 @@
         <v>39</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C31">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F31">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G31">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J31">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1515,31 +1515,31 @@
         <v>40</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E32">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
       <c r="G32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H32">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J32">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1547,31 +1547,31 @@
         <v>41</v>
       </c>
       <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
         <v>9</v>
       </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33">
-        <v>4</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
       <c r="G33">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H33">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1579,28 +1579,28 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D34">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G34">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H34">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J34">
         <v>4</v>
@@ -1611,31 +1611,31 @@
         <v>43</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>5</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1643,31 +1643,31 @@
         <v>44</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E36">
         <v>8</v>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G36">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H36">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1675,28 +1675,28 @@
         <v>45</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G37">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -1707,31 +1707,31 @@
         <v>46</v>
       </c>
       <c r="B38">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G38">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I38">
         <v>1</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalize version to deliver reports to user
</commit_message>
<xml_diff>
--- a/Data/Call/Call_CBU.xlsx
+++ b/Data/Call/Call_CBU.xlsx
@@ -588,31 +588,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="C2">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="D2">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="E2">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F2">
-        <v>230</v>
+        <v>274</v>
       </c>
       <c r="G2">
-        <v>269</v>
+        <v>369</v>
       </c>
       <c r="H2">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="I2">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="J2">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -620,31 +620,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H3">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -652,7 +652,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -661,22 +661,22 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -684,31 +684,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -716,31 +716,31 @@
         <v>14</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>6</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -748,31 +748,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <v>12</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -780,31 +780,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8">
         <v>4</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -812,31 +812,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>39</v>
+      </c>
+      <c r="G9">
+        <v>58</v>
+      </c>
+      <c r="H9">
+        <v>36</v>
+      </c>
+      <c r="I9">
+        <v>15</v>
+      </c>
+      <c r="J9">
         <v>26</v>
-      </c>
-      <c r="E9">
-        <v>23</v>
-      </c>
-      <c r="F9">
-        <v>47</v>
-      </c>
-      <c r="G9">
-        <v>62</v>
-      </c>
-      <c r="H9">
-        <v>41</v>
-      </c>
-      <c r="I9">
-        <v>10</v>
-      </c>
-      <c r="J9">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -844,31 +844,31 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>17</v>
       </c>
       <c r="G10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -876,31 +876,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H11">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -911,28 +911,28 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -940,31 +940,31 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -975,28 +975,28 @@
         <v>6</v>
       </c>
       <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
         <v>6</v>
       </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
       <c r="E14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>8</v>
       </c>
       <c r="G14">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
         <v>6</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1004,31 +1004,31 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D15">
+        <v>48</v>
+      </c>
+      <c r="E15">
         <v>22</v>
       </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
       <c r="F15">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="G15">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="H15">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J15">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1036,31 +1036,31 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>21</v>
+      </c>
+      <c r="H16">
+        <v>21</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
         <v>8</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>17</v>
-      </c>
-      <c r="G16">
-        <v>20</v>
-      </c>
-      <c r="H16">
-        <v>17</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1068,31 +1068,31 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1100,31 +1100,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1132,31 +1132,31 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1164,31 +1164,31 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1199,28 +1199,28 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
       <c r="G21">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H21">
         <v>6</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J21">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1228,31 +1228,31 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D22">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G22">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H22">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J22">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1260,31 +1260,31 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>10</v>
       </c>
       <c r="G23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>6</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1292,31 +1292,31 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>2</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1324,31 +1324,31 @@
         <v>33</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
         <v>8</v>
       </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
       <c r="G25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H25">
         <v>7</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J25">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1356,13 +1356,13 @@
         <v>34</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1374,13 +1374,13 @@
         <v>3</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J26">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1388,31 +1388,31 @@
         <v>35</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <v>9</v>
       </c>
       <c r="H27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1420,25 +1420,25 @@
         <v>36</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F28">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H28">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1452,31 +1452,31 @@
         <v>37</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F29">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G29">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="H29">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1516,10 +1516,10 @@
         <v>39</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -1528,19 +1528,19 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1548,31 +1548,31 @@
         <v>40</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1612,31 +1612,31 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H34">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1650,25 +1650,25 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>3</v>
       </c>
       <c r="H35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1676,31 +1676,31 @@
         <v>44</v>
       </c>
       <c r="B36">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C36">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D36">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E36">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F36">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="G36">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="H36">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="I36">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J36">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1714,16 +1714,16 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1740,31 +1740,31 @@
         <v>46</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J38">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1772,31 +1772,31 @@
         <v>47</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F39">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G39">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1804,31 +1804,31 @@
         <v>48</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I40">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1839,28 +1839,28 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H41">
         <v>2</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1868,31 +1868,31 @@
         <v>50</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H42">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J42">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1900,31 +1900,31 @@
         <v>51</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G43">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1932,31 +1932,31 @@
         <v>52</v>
       </c>
       <c r="B44">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D44">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E44">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F44">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G44">
+        <v>37</v>
+      </c>
+      <c r="H44">
+        <v>19</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
         <v>22</v>
-      </c>
-      <c r="H44">
-        <v>16</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1964,31 +1964,31 @@
         <v>53</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1996,19 +1996,19 @@
         <v>54</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D46">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G46">
         <v>9</v>
@@ -2017,10 +2017,10 @@
         <v>5</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2028,31 +2028,31 @@
         <v>55</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2060,28 +2060,28 @@
         <v>56</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -2092,31 +2092,31 @@
         <v>57</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H49">
         <v>3</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J49">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>